<commit_message>
relazione fatta fino a dati raccolti
</commit_message>
<xml_diff>
--- a/CALORIMETRO/calorimetro.xlsx
+++ b/CALORIMETRO/calorimetro.xlsx
@@ -6,17 +6,18 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="preliminari" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="T1=20 T2=50" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="t_metallo = 100 t_calorimetr=20" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="condizioni di partenza" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="parte A" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="parte B" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="parte C" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="parte D" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>m_beker</t>
   </si>
@@ -60,9 +61,21 @@
     <t>200g</t>
   </si>
   <si>
+    <t>T_ambiente</t>
+  </si>
+  <si>
+    <t>20°C</t>
+  </si>
+  <si>
     <t>TE</t>
   </si>
   <si>
+    <t xml:space="preserve">T acqua ambiente (°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T acqua calda (°C)</t>
+  </si>
+  <si>
     <t>materiale</t>
   </si>
   <si>
@@ -81,6 +94,15 @@
     <t xml:space="preserve">AVG TE</t>
   </si>
   <si>
+    <t xml:space="preserve">T metallo (°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T acqua (°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m acqua (g)</t>
+  </si>
+  <si>
     <t>ottone</t>
   </si>
   <si>
@@ -90,16 +112,25 @@
     <t>alluminio</t>
   </si>
   <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V = 15V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I = 3.5A</t>
+    <t xml:space="preserve">t (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T (°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V (volt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I (Ampere)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m ghiaccio (g)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T ghiaccio (°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T equilibrio</t>
   </si>
 </sst>
 </file>
@@ -107,14 +138,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="160" formatCode="0.0"/>
+    <numFmt numFmtId="160" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,12 +173,24 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="4" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +491,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="New Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -475,15 +523,15 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface="Arial"/>
         <a:cs typeface="Arial"/>
       </a:majorFont>
@@ -502,76 +550,69 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -607,38 +648,45 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -649,6 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -656,68 +708,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.421875"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="21.433571428571426"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="12.43357142857143"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" t="s">
+    <row r="1" ht="17.25" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="14.25">
-      <c r="A2" t="s">
+    <row r="2" ht="17.25" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
-      <c r="A3" t="s">
+    <row r="3" ht="17.25" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="14.25">
-      <c r="A5" t="s">
+    <row r="4" ht="17.25" customHeight="1">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" ht="17.25" customHeight="1">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" ht="14.25">
-      <c r="A6" t="s">
+    <row r="6" ht="17.25" customHeight="1">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="14.25">
-      <c r="A7" t="s">
+    <row r="7" ht="17.25" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" ht="14.25">
-      <c r="A9" t="s">
+    <row r="8" ht="17.25" customHeight="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" ht="17.25" customHeight="1">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10" ht="17.25" customHeight="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" ht="17.25" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
@@ -725,46 +798,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="3" width="21.433571428571426"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="3" width="16.147857142857141"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25">
-      <c r="A2">
+    <row r="1" ht="17.25" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" ht="17.25" customHeight="1">
+      <c r="A2" s="4">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3">
+      <c r="B2" s="4">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1">
+      <c r="A3" s="4">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" ht="17.25" customHeight="1">
+      <c r="A4" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" ht="17.25" customHeight="1">
+      <c r="A5" s="4">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" ht="17.25" customHeight="1">
+      <c r="A6" s="4">
         <v>34</v>
       </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
@@ -772,102 +874,129 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="3" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="3" max="5" style="5" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" style="6" width="12.43357142857143"/>
+    <col bestFit="1" min="7" max="7" width="12.421875"/>
+    <col bestFit="1" min="8" max="8" width="11.09375"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
+    <row r="1" ht="17.25" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" ht="14.25">
-      <c r="A2" t="s">
+      <c r="C1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" ht="17.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4">
         <v>122</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="7">
         <v>23</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="7">
         <v>23.5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="7">
         <v>23.5</v>
       </c>
-      <c r="F2" s="3">
-        <f>AVERAGE(C2:E2)</f>
+      <c r="F2" s="8">
+        <f t="shared" ref="F2:F4" si="0">AVERAGE(C2:E2)</f>
         <v>23.333333333333332</v>
       </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4">
         <v>128</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="7">
         <v>24</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="7">
         <v>23.5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="7">
         <v>24</v>
       </c>
-      <c r="F3" s="3">
-        <f>AVERAGE(C3:E3)</f>
+      <c r="F3" s="8">
+        <f t="shared" si="0"/>
         <v>23.833333333333332</v>
       </c>
     </row>
-    <row r="4" ht="14.25">
-      <c r="A4" t="s">
-        <v>23</v>
+    <row r="4" ht="17.25" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B4" s="4">
         <v>39</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="7">
         <v>22.5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="7">
         <v>23</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="7">
         <v>23</v>
       </c>
-      <c r="F4" s="3">
-        <f>AVERAGE(C4:E4)</f>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
         <v>22.833333333333332</v>
       </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
@@ -875,155 +1004,257 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="3" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="6" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="3" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="6" width="12.43357142857143"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="17.25" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" ht="17.25" customHeight="1">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>21.5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" ht="17.25" customHeight="1">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>22.5</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" ht="17.25" customHeight="1">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" ht="17.25" customHeight="1">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>23.5</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" ht="17.25" customHeight="1">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" ht="17.25" customHeight="1">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>24.5</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" ht="17.25" customHeight="1">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" ht="17.25" customHeight="1">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" ht="17.25" customHeight="1">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" ht="17.25" customHeight="1">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" ht="17.25" customHeight="1">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7">
+        <v>29.5</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" ht="17.25" customHeight="1">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7">
+        <v>30.5</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" ht="17.25" customHeight="1">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" ht="17.25" customHeight="1">
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" ht="17.25" customHeight="1">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7">
+        <v>35.5</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="6"/>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="10.90234375"/>
+    <col bestFit="1" min="2" max="2" width="12.61328125"/>
+    <col bestFit="1" min="3" max="3" width="16.140625"/>
+    <col bestFit="1" min="4" max="4" width="12.8125"/>
+    <col bestFit="1" min="5" max="5" width="10.5234375"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-      <c r="I1">
-        <v>7</v>
-      </c>
-      <c r="J1">
-        <v>8</v>
-      </c>
-      <c r="K1">
-        <v>9</v>
-      </c>
-      <c r="L1">
-        <v>10</v>
-      </c>
-      <c r="M1">
-        <v>11</v>
-      </c>
-      <c r="N1">
-        <v>12</v>
-      </c>
-      <c r="O1">
-        <v>13</v>
-      </c>
-      <c r="P1">
-        <v>14</v>
-      </c>
-      <c r="Q1">
-        <v>15</v>
-      </c>
-      <c r="R1">
-        <v>16</v>
-      </c>
-      <c r="S1">
-        <v>17</v>
-      </c>
-      <c r="T1">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="U1">
-        <v>19</v>
-      </c>
-      <c r="V1">
-        <v>20</v>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>25</v>
+      <c r="A2">
+        <v>300</v>
       </c>
       <c r="B2">
-        <v>21.5</v>
+        <v>50</v>
       </c>
       <c r="C2">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="D2">
-        <v>22.5</v>
+        <v>-17</v>
       </c>
       <c r="E2">
-        <v>23</v>
-      </c>
-      <c r="F2">
-        <v>23.5</v>
-      </c>
-      <c r="G2">
-        <v>24</v>
-      </c>
-      <c r="H2">
-        <v>24.5</v>
-      </c>
-      <c r="I2">
-        <v>25</v>
-      </c>
-      <c r="J2">
-        <v>26</v>
-      </c>
-      <c r="K2">
-        <v>27</v>
-      </c>
-      <c r="L2">
-        <v>28</v>
-      </c>
-      <c r="M2">
-        <v>29.5</v>
-      </c>
-      <c r="N2">
-        <v>30.5</v>
-      </c>
-      <c r="O2">
-        <v>32</v>
-      </c>
-      <c r="P2">
-        <v>34</v>
-      </c>
-      <c r="Q2">
-        <v>35.5</v>
-      </c>
-      <c r="R2">
-        <v>37</v>
-      </c>
-      <c r="S2">
-        <v>39</v>
-      </c>
-      <c r="T2">
-        <v>40.5</v>
-      </c>
-      <c r="U2">
-        <v>43</v>
-      </c>
-      <c r="V2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
+        <v>57.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>